<commit_message>
[#13] Update FormData ID in BulkUploadDataTestCase to avoid conflicts
</commit_message>
<xml_diff>
--- a/backend/api/v1/v1_jobs/tests/fixtures/test-success-new-monitoring.xlsx
+++ b/backend/api/v1/v1_jobs/tests/fixtures/test-success-new-monitoring.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="questions" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="options" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="data" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="questions" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="options" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -390,13 +390,17 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -416,15 +420,121 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:X1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -503,62 +613,62 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" s="0" t="n">
+    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>9999</v>
+      </c>
+      <c r="C2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="J2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="0" t="s">
+      <c r="L2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="2" t="n">
         <v>23911</v>
       </c>
-      <c r="N2" s="0" t="s">
+      <c r="N2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="0" t="s">
+      <c r="O2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="0" t="s">
+      <c r="P2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="R2" s="0" t="s">
+      <c r="R2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="S2" s="2" t="n">
         <v>5.6</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="T2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="W2" s="0" t="s">
+      <c r="W2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="X2" s="0" t="s">
+      <c r="X2" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -578,7 +688,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -611,215 +721,215 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="0" t="s">
+      <c r="D16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>68</v>
       </c>
     </row>
@@ -835,7 +945,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -859,145 +969,145 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="2" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>